<commit_message>
season of birth changes
</commit_message>
<xml_diff>
--- a/Arduino-Leonardo/Analysis/Season-of-Birth/Ptpt_ID_Links.xlsx
+++ b/Arduino-Leonardo/Analysis/Season-of-Birth/Ptpt_ID_Links.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="473" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC7C28AE-1CA0-4E02-A291-B45C99FD35BB}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dturner\Documents\GitHub\ICVS-Code\Arduino-Leonardo\Analysis\Season-of-Birth\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10800"/>
   </bookViews>
   <sheets>
     <sheet name="Merged" sheetId="1" r:id="rId1"/>
     <sheet name="Regan&amp;Hexley" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -502,9 +506,6 @@
     <t>BBE</t>
   </si>
   <si>
-    <t>DAM / JBM</t>
-  </si>
-  <si>
     <t>Shameer Ponsla</t>
   </si>
   <si>
@@ -1400,13 +1401,16 @@
   </si>
   <si>
     <t>ADP</t>
+  </si>
+  <si>
+    <t>JBM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1923,14 +1927,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" style="21" customWidth="1"/>
@@ -1940,7 +1944,7 @@
     <col min="6" max="7" width="5.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1960,7 +1964,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="16"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
@@ -1977,7 +1981,7 @@
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
@@ -1994,7 +1998,7 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
@@ -2013,7 +2017,7 @@
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>12</v>
       </c>
@@ -2032,7 +2036,7 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -2049,7 +2053,7 @@
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -2066,7 +2070,7 @@
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>19</v>
       </c>
@@ -2083,7 +2087,7 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>21</v>
       </c>
@@ -2100,7 +2104,7 @@
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>23</v>
       </c>
@@ -2119,7 +2123,7 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>26</v>
       </c>
@@ -2136,7 +2140,7 @@
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>28</v>
       </c>
@@ -2153,7 +2157,7 @@
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>30</v>
       </c>
@@ -2170,7 +2174,7 @@
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>32</v>
       </c>
@@ -2187,7 +2191,7 @@
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>34</v>
       </c>
@@ -2204,7 +2208,7 @@
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>36</v>
       </c>
@@ -2221,7 +2225,7 @@
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>38</v>
       </c>
@@ -2242,7 +2246,7 @@
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>42</v>
       </c>
@@ -2261,7 +2265,7 @@
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>45</v>
       </c>
@@ -2278,7 +2282,7 @@
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>47</v>
       </c>
@@ -2295,7 +2299,7 @@
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>49</v>
       </c>
@@ -2312,7 +2316,7 @@
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>51</v>
       </c>
@@ -2329,7 +2333,7 @@
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>53</v>
       </c>
@@ -2346,7 +2350,7 @@
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>55</v>
       </c>
@@ -2365,7 +2369,7 @@
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>58</v>
       </c>
@@ -2382,7 +2386,7 @@
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>60</v>
       </c>
@@ -2399,7 +2403,7 @@
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>62</v>
       </c>
@@ -2416,7 +2420,7 @@
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>64</v>
       </c>
@@ -2433,7 +2437,7 @@
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>66</v>
       </c>
@@ -2452,7 +2456,7 @@
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>69</v>
       </c>
@@ -2469,7 +2473,7 @@
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>71</v>
       </c>
@@ -2486,7 +2490,7 @@
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>73</v>
       </c>
@@ -2503,7 +2507,7 @@
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>75</v>
       </c>
@@ -2520,7 +2524,7 @@
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>77</v>
       </c>
@@ -2537,7 +2541,7 @@
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>79</v>
       </c>
@@ -2556,7 +2560,7 @@
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>82</v>
       </c>
@@ -2573,7 +2577,7 @@
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>84</v>
       </c>
@@ -2590,7 +2594,7 @@
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>86</v>
       </c>
@@ -2609,7 +2613,7 @@
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>89</v>
       </c>
@@ -2626,7 +2630,7 @@
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>91</v>
       </c>
@@ -2643,7 +2647,7 @@
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>93</v>
       </c>
@@ -2660,7 +2664,7 @@
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>95</v>
       </c>
@@ -2677,7 +2681,7 @@
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>97</v>
       </c>
@@ -2694,7 +2698,7 @@
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>99</v>
       </c>
@@ -2711,7 +2715,7 @@
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>101</v>
       </c>
@@ -2728,7 +2732,7 @@
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>103</v>
       </c>
@@ -2747,7 +2751,7 @@
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>106</v>
       </c>
@@ -2768,7 +2772,7 @@
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>110</v>
       </c>
@@ -2785,7 +2789,7 @@
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>112</v>
       </c>
@@ -2802,7 +2806,7 @@
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>114</v>
       </c>
@@ -2819,7 +2823,7 @@
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>116</v>
       </c>
@@ -2836,7 +2840,7 @@
       <c r="G51" s="6"/>
       <c r="H51" s="6"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>118</v>
       </c>
@@ -2855,7 +2859,7 @@
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>121</v>
       </c>
@@ -2872,7 +2876,7 @@
       <c r="G53" s="6"/>
       <c r="H53" s="6"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>123</v>
       </c>
@@ -2889,7 +2893,7 @@
       <c r="G54" s="6"/>
       <c r="H54" s="6"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>125</v>
       </c>
@@ -2906,7 +2910,7 @@
       <c r="G55" s="6"/>
       <c r="H55" s="6"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>127</v>
       </c>
@@ -2923,7 +2927,7 @@
       <c r="G56" s="6"/>
       <c r="H56" s="6"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>129</v>
       </c>
@@ -2940,7 +2944,7 @@
       <c r="G57" s="6"/>
       <c r="H57" s="6"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
         <v>131</v>
       </c>
@@ -2957,7 +2961,7 @@
       <c r="G58" s="6"/>
       <c r="H58" s="6"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>133</v>
       </c>
@@ -2974,7 +2978,7 @@
       <c r="G59" s="6"/>
       <c r="H59" s="6"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>135</v>
       </c>
@@ -2991,7 +2995,7 @@
       <c r="G60" s="6"/>
       <c r="H60" s="6"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>137</v>
       </c>
@@ -3008,7 +3012,7 @@
       <c r="G61" s="6"/>
       <c r="H61" s="6"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>139</v>
       </c>
@@ -3025,7 +3029,7 @@
       <c r="G62" s="6"/>
       <c r="H62" s="6"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>141</v>
       </c>
@@ -3042,7 +3046,7 @@
       <c r="G63" s="6"/>
       <c r="H63" s="6"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>143</v>
       </c>
@@ -3059,7 +3063,7 @@
       <c r="G64" s="6"/>
       <c r="H64" s="6"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>145</v>
       </c>
@@ -3076,7 +3080,7 @@
       <c r="G65" s="6"/>
       <c r="H65" s="6"/>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>147</v>
       </c>
@@ -3093,7 +3097,7 @@
       <c r="G66" s="6"/>
       <c r="H66" s="6"/>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>149</v>
       </c>
@@ -3112,7 +3116,7 @@
       <c r="G67" s="6"/>
       <c r="H67" s="6"/>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>152</v>
       </c>
@@ -3129,7 +3133,7 @@
       <c r="G68" s="6"/>
       <c r="H68" s="6"/>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>154</v>
       </c>
@@ -3141,16 +3145,16 @@
         <v>155</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>156</v>
+        <v>455</v>
       </c>
       <c r="E69" s="9"/>
       <c r="F69" s="6"/>
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B70" s="19" t="str">
         <f>IF(ISNA(VLOOKUP(A70,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE)),"",VLOOKUP(A70,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE))</f>
@@ -3158,16 +3162,16 @@
       </c>
       <c r="C70" s="9"/>
       <c r="D70" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E70" s="9"/>
       <c r="F70" s="6"/>
       <c r="G70" s="6"/>
       <c r="H70" s="6"/>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B71" s="19" t="str">
         <f>IF(ISNA(VLOOKUP(A71,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE)),"",VLOOKUP(A71,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE))</f>
@@ -3175,23 +3179,23 @@
       </c>
       <c r="C71" s="9"/>
       <c r="D71" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E71" s="9"/>
       <c r="F71" s="6"/>
       <c r="G71" s="6"/>
       <c r="H71" s="6"/>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B72" s="19" t="str">
         <f>IF(ISNA(VLOOKUP(A72,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE)),"",VLOOKUP(A72,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE))</f>
         <v/>
       </c>
       <c r="C72" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D72" s="9"/>
       <c r="E72" s="9"/>
@@ -3199,9 +3203,9 @@
       <c r="G72" s="6"/>
       <c r="H72" s="6"/>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B73" s="19" t="str">
         <f>IF(ISNA(VLOOKUP(A73,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE)),"",VLOOKUP(A73,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE))</f>
@@ -3209,16 +3213,16 @@
       </c>
       <c r="C73" s="9"/>
       <c r="D73" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E73" s="9"/>
       <c r="F73" s="6"/>
       <c r="G73" s="6"/>
       <c r="H73" s="6"/>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B74" s="19" t="str">
         <f>IF(ISNA(VLOOKUP(A74,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE)),"",VLOOKUP(A74,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE))</f>
@@ -3226,16 +3230,16 @@
       </c>
       <c r="C74" s="9"/>
       <c r="D74" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E74" s="9"/>
       <c r="F74" s="6"/>
       <c r="G74" s="6"/>
       <c r="H74" s="6"/>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B75" s="19" t="str">
         <f>IF(ISNA(VLOOKUP(A75,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE)),"",VLOOKUP(A75,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE))</f>
@@ -3244,15 +3248,15 @@
       <c r="C75" s="9"/>
       <c r="D75" s="9"/>
       <c r="E75" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F75" s="6"/>
       <c r="G75" s="6"/>
       <c r="H75" s="6"/>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B76" s="19" t="str">
         <f>IF(ISNA(VLOOKUP(A76,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE)),"",VLOOKUP(A76,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE))</f>
@@ -3260,16 +3264,16 @@
       </c>
       <c r="C76" s="9"/>
       <c r="D76" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E76" s="9"/>
       <c r="F76" s="6"/>
       <c r="G76" s="6"/>
       <c r="H76" s="6"/>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B77" s="19" t="str">
         <f>IF(ISNA(VLOOKUP(A77,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE)),"",VLOOKUP(A77,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE))</f>
@@ -3277,16 +3281,16 @@
       </c>
       <c r="C77" s="9"/>
       <c r="D77" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E77" s="9"/>
       <c r="F77" s="6"/>
       <c r="G77" s="6"/>
       <c r="H77" s="6"/>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B78" s="19" t="str">
         <f>IF(ISNA(VLOOKUP(A78,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE)),"",VLOOKUP(A78,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE))</f>
@@ -3294,16 +3298,16 @@
       </c>
       <c r="C78" s="9"/>
       <c r="D78" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E78" s="9"/>
       <c r="F78" s="6"/>
       <c r="G78" s="6"/>
       <c r="H78" s="6"/>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B79" s="19" t="str">
         <f>IF(ISNA(VLOOKUP(A79,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE)),"",VLOOKUP(A79,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE))</f>
@@ -3312,22 +3316,22 @@
       <c r="C79" s="9"/>
       <c r="D79" s="9"/>
       <c r="E79" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F79" s="6"/>
       <c r="G79" s="6"/>
       <c r="H79" s="6"/>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B80" s="19" t="str">
         <f>IF(ISNA(VLOOKUP(A80,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE)),"",VLOOKUP(A80,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE))</f>
         <v/>
       </c>
       <c r="C80" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D80" s="9"/>
       <c r="E80" s="9"/>
@@ -3335,9 +3339,9 @@
       <c r="G80" s="6"/>
       <c r="H80" s="6"/>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B81" s="19" t="str">
         <f>IF(ISNA(VLOOKUP(A81,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE)),"",VLOOKUP(A81,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE))</f>
@@ -3346,15 +3350,15 @@
       <c r="C81" s="9"/>
       <c r="D81" s="9"/>
       <c r="E81" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F81" s="6"/>
       <c r="G81" s="6"/>
       <c r="H81" s="6"/>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B82" s="19" t="str">
         <f>IF(ISNA(VLOOKUP(A82,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE)),"",VLOOKUP(A82,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE))</f>
@@ -3362,16 +3366,16 @@
       </c>
       <c r="C82" s="9"/>
       <c r="D82" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E82" s="9"/>
       <c r="F82" s="6"/>
       <c r="G82" s="6"/>
       <c r="H82" s="6"/>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B83" s="19" t="str">
         <f>IF(ISNA(VLOOKUP(A83,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE)),"",VLOOKUP(A83,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE))</f>
@@ -3379,23 +3383,23 @@
       </c>
       <c r="C83" s="9"/>
       <c r="D83" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E83" s="9"/>
       <c r="F83" s="6"/>
       <c r="G83" s="6"/>
       <c r="H83" s="6"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B84" s="19" t="str">
         <f>IF(ISNA(VLOOKUP(A84,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE)),"",VLOOKUP(A84,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE))</f>
         <v/>
       </c>
       <c r="C84" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D84" s="9"/>
       <c r="E84" s="9"/>
@@ -3403,9 +3407,9 @@
       <c r="G84" s="6"/>
       <c r="H84" s="6"/>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B85" s="19" t="str">
         <f>IF(ISNA(VLOOKUP(A85,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE)),"",VLOOKUP(A85,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE))</f>
@@ -3413,16 +3417,16 @@
       </c>
       <c r="C85" s="9"/>
       <c r="D85" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E85" s="9"/>
       <c r="F85" s="6"/>
       <c r="G85" s="6"/>
       <c r="H85" s="6"/>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B86" s="19" t="str">
         <f>IF(ISNA(VLOOKUP(A86,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE)),"",VLOOKUP(A86,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE))</f>
@@ -3431,22 +3435,22 @@
       <c r="C86" s="9"/>
       <c r="D86" s="9"/>
       <c r="E86" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F86" s="6"/>
       <c r="G86" s="6"/>
       <c r="H86" s="6"/>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B87" s="19" t="str">
         <f>IF(ISNA(VLOOKUP(A87,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE)),"",VLOOKUP(A87,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE))</f>
         <v/>
       </c>
       <c r="C87" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D87" s="9"/>
       <c r="E87" s="9"/>
@@ -3454,16 +3458,16 @@
       <c r="G87" s="6"/>
       <c r="H87" s="6"/>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B88" s="19" t="str">
         <f>IF(ISNA(VLOOKUP(A88,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE)),"",VLOOKUP(A88,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE))</f>
         <v/>
       </c>
       <c r="C88" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D88" s="9"/>
       <c r="E88" s="9"/>
@@ -3471,9 +3475,9 @@
       <c r="G88" s="6"/>
       <c r="H88" s="6"/>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B89" s="19" t="str">
         <f>IF(ISNA(VLOOKUP(A89,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE)),"",VLOOKUP(A89,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE))</f>
@@ -3481,16 +3485,16 @@
       </c>
       <c r="C89" s="9"/>
       <c r="D89" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E89" s="9"/>
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
       <c r="H89" s="6"/>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B90" s="19" t="str">
         <f>IF(ISNA(VLOOKUP(A90,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE)),"",VLOOKUP(A90,'Regan&amp;Hexley'!$A$1:$C$95,3,FALSE))</f>
@@ -3499,314 +3503,314 @@
       <c r="C90" s="9"/>
       <c r="D90" s="9"/>
       <c r="E90" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
       <c r="H90" s="6"/>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="20"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="20"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="20"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="20"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="20"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="20"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="20"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="20"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="20"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="20"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="20"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="20"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="20"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="20"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="20"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="20"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="20"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="20"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
     </row>
-    <row r="109" spans="1:5">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="20"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="20"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="20"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="20"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="20"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
     </row>
-    <row r="114" spans="1:5">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="20"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="20"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="20"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="20"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="20"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="20"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="20"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="20"/>
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="20"/>
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="20"/>
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="20"/>
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="20"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="20"/>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="20"/>
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="20"/>
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="20"/>
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="20"/>
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="20"/>
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="20"/>
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="20"/>
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
     </row>
-    <row r="134" spans="1:5">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="20"/>
       <c r="C134" s="1"/>
@@ -3819,1101 +3823,1101 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E0ADF7-511A-4A0F-93A9-17173D9FA569}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C95"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="I84" sqref="I84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="C1" s="23" t="s">
         <v>200</v>
       </c>
-      <c r="C1" s="23" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="C2" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="C2" s="23" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
         <v>203</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="23" t="s">
-        <v>204</v>
       </c>
       <c r="B3" s="23"/>
       <c r="C3" s="23" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="23" t="s">
+      <c r="B4" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="C4" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="C4" s="23" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="23" t="s">
+      <c r="B5" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="C5" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="C5" s="23" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="23" t="s">
+      <c r="B6" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="C6" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="C6" s="23" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="23" t="s">
+      <c r="B7" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="C7" s="23" t="s">
         <v>216</v>
       </c>
-      <c r="C7" s="23" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="23" t="s">
+      <c r="B8" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="C8" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="C8" s="23" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="23" t="s">
+      <c r="B9" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="C9" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="C9" s="23" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="23" t="s">
+      <c r="B10" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="C10" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="C10" s="23" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="23" t="s">
+      <c r="B11" s="17" t="s">
         <v>227</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="C11" s="23" t="s">
         <v>228</v>
       </c>
-      <c r="C11" s="23" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
         <v>229</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="23" t="s">
-        <v>230</v>
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="23" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="23" t="s">
+      <c r="B13" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="C13" s="23" t="s">
         <v>233</v>
       </c>
-      <c r="C13" s="23" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
         <v>234</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="23" t="s">
-        <v>235</v>
       </c>
       <c r="B14" s="23"/>
       <c r="C14" s="23" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
         <v>236</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="23" t="s">
-        <v>237</v>
       </c>
       <c r="B15" s="23"/>
       <c r="C15" s="23" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="23" t="s">
+      <c r="B16" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="C16" s="23" t="s">
         <v>240</v>
       </c>
-      <c r="C16" s="23" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="23" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="23" t="s">
+      <c r="B17" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="C17" s="23" t="s">
         <v>243</v>
       </c>
-      <c r="C17" s="23" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="23" t="s">
+      <c r="B18" s="17" t="s">
         <v>245</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="C18" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="C18" s="23" t="s">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="23" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="23" t="s">
+      <c r="B19" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="C19" s="23" t="s">
         <v>249</v>
       </c>
-      <c r="C19" s="23" t="s">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="23" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="23" t="s">
+      <c r="B20" s="17" t="s">
         <v>251</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="C20" s="23" t="s">
         <v>252</v>
       </c>
-      <c r="C20" s="23" t="s">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="23" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="23" t="s">
+      <c r="B21" s="17" t="s">
         <v>254</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="C21" s="23" t="s">
         <v>255</v>
       </c>
-      <c r="C21" s="23" t="s">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="23" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="23" t="s">
+      <c r="B22" s="17" t="s">
         <v>257</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="C22" s="23" t="s">
         <v>258</v>
       </c>
-      <c r="C22" s="23" t="s">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="B23" s="17" t="s">
+      <c r="C23" s="23" t="s">
         <v>260</v>
       </c>
-      <c r="C23" s="23" t="s">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="23" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="23" t="s">
+      <c r="B24" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="C24" s="23" t="s">
         <v>263</v>
       </c>
-      <c r="C24" s="23" t="s">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="23" t="s">
         <v>264</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="23" t="s">
-        <v>265</v>
       </c>
       <c r="B25" s="23"/>
       <c r="C25" s="23" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="23" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="23" t="s">
+      <c r="B26" s="17" t="s">
         <v>267</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="C26" s="23" t="s">
         <v>268</v>
       </c>
-      <c r="C26" s="23" t="s">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="23" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="23" t="s">
+      <c r="B27" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="C27" s="23" t="s">
         <v>271</v>
       </c>
-      <c r="C27" s="23" t="s">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="23" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="23" t="s">
+      <c r="B28" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="C28" s="23" t="s">
         <v>274</v>
       </c>
-      <c r="C28" s="23" t="s">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="23" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="23" t="s">
+      <c r="B29" s="17" t="s">
         <v>276</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="C29" s="23" t="s">
         <v>277</v>
       </c>
-      <c r="C29" s="23" t="s">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="23" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="23" t="s">
+      <c r="B30" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="C30" s="23" t="s">
         <v>280</v>
       </c>
-      <c r="C30" s="23" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="23"/>
       <c r="B31" s="23"/>
       <c r="C31" s="23" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="23" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="23" t="s">
+      <c r="B32" s="17" t="s">
         <v>283</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="C32" s="23" t="s">
         <v>284</v>
       </c>
-      <c r="C32" s="23" t="s">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="23" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="23" t="s">
+      <c r="B33" s="17" t="s">
         <v>286</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="C33" s="23" t="s">
         <v>287</v>
       </c>
-      <c r="C33" s="23" t="s">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="23" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="23" t="s">
+      <c r="B34" s="17" t="s">
         <v>289</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="C34" s="23" t="s">
         <v>290</v>
       </c>
-      <c r="C34" s="23" t="s">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="23" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="23" t="s">
+      <c r="B35" s="17" t="s">
         <v>292</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="C35" s="23" t="s">
         <v>293</v>
       </c>
-      <c r="C35" s="23" t="s">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="23" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="23" t="s">
+      <c r="B36" s="17" t="s">
         <v>295</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="C36" s="23" t="s">
         <v>296</v>
       </c>
-      <c r="C36" s="23" t="s">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="23" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="23" t="s">
+      <c r="B37" s="17" t="s">
         <v>298</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="C37" s="23" t="s">
         <v>299</v>
       </c>
-      <c r="C37" s="23" t="s">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="23" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="23" t="s">
+      <c r="B38" s="17" t="s">
         <v>301</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="C38" s="23" t="s">
         <v>302</v>
       </c>
-      <c r="C38" s="23" t="s">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="23" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="23" t="s">
+      <c r="B39" s="17" t="s">
         <v>304</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="C39" s="23" t="s">
         <v>305</v>
       </c>
-      <c r="C39" s="23" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="23"/>
       <c r="B40" s="23"/>
       <c r="C40" s="23" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="23" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="23" t="s">
+      <c r="B41" s="17" t="s">
         <v>308</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="C41" s="23" t="s">
         <v>309</v>
       </c>
-      <c r="C41" s="23" t="s">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="23" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="23" t="s">
+      <c r="B42" s="17" t="s">
         <v>311</v>
       </c>
-      <c r="B42" s="17" t="s">
+      <c r="C42" s="23" t="s">
         <v>312</v>
       </c>
-      <c r="C42" s="23" t="s">
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="23" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="23" t="s">
+      <c r="B43" s="17" t="s">
         <v>314</v>
       </c>
-      <c r="B43" s="17" t="s">
+      <c r="C43" s="23" t="s">
         <v>315</v>
       </c>
-      <c r="C43" s="23" t="s">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="23" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="23" t="s">
+      <c r="B44" s="17" t="s">
         <v>317</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="C44" s="23" t="s">
         <v>318</v>
       </c>
-      <c r="C44" s="23" t="s">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="23" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="23" t="s">
+      <c r="B45" s="17" t="s">
         <v>320</v>
       </c>
-      <c r="B45" s="17" t="s">
+      <c r="C45" s="23" t="s">
         <v>321</v>
       </c>
-      <c r="C45" s="23" t="s">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="23" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="23" t="s">
+      <c r="B46" s="17" t="s">
         <v>323</v>
       </c>
-      <c r="B46" s="17" t="s">
+      <c r="C46" s="23" t="s">
         <v>324</v>
       </c>
-      <c r="C46" s="23" t="s">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="23" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="23" t="s">
+      <c r="B47" s="17" t="s">
         <v>326</v>
       </c>
-      <c r="B47" s="17" t="s">
+      <c r="C47" s="23" t="s">
         <v>327</v>
       </c>
-      <c r="C47" s="23" t="s">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="23" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="23" t="s">
+      <c r="B48" s="17" t="s">
         <v>329</v>
       </c>
-      <c r="B48" s="17" t="s">
+      <c r="C48" s="23" t="s">
         <v>330</v>
       </c>
-      <c r="C48" s="23" t="s">
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="23" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="23" t="s">
+      <c r="B49" s="17" t="s">
         <v>332</v>
       </c>
-      <c r="B49" s="17" t="s">
+      <c r="C49" s="23" t="s">
         <v>333</v>
       </c>
-      <c r="C49" s="23" t="s">
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="23" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="23" t="s">
+      <c r="B50" s="17" t="s">
         <v>335</v>
       </c>
-      <c r="B50" s="17" t="s">
+      <c r="C50" s="23" t="s">
         <v>336</v>
       </c>
-      <c r="C50" s="23" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="23"/>
       <c r="B51" s="23"/>
       <c r="C51" s="23" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="23" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="23" t="s">
+      <c r="B52" s="17" t="s">
         <v>339</v>
       </c>
-      <c r="B52" s="17" t="s">
+      <c r="C52" s="23" t="s">
         <v>340</v>
       </c>
-      <c r="C52" s="23" t="s">
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="23" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="23" t="s">
+      <c r="B53" s="17" t="s">
         <v>342</v>
       </c>
-      <c r="B53" s="17" t="s">
+      <c r="C53" s="23" t="s">
         <v>343</v>
       </c>
-      <c r="C53" s="23" t="s">
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="23" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="23" t="s">
+      <c r="B54" s="17" t="s">
         <v>345</v>
       </c>
-      <c r="B54" s="17" t="s">
+      <c r="C54" s="23" t="s">
         <v>346</v>
       </c>
-      <c r="C54" s="23" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="23" t="s">
         <v>97</v>
       </c>
       <c r="B55" s="17" t="s">
+        <v>347</v>
+      </c>
+      <c r="C55" s="23" t="s">
         <v>348</v>
       </c>
-      <c r="C55" s="23" t="s">
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="23" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="23" t="s">
+      <c r="B56" s="17" t="s">
         <v>350</v>
       </c>
-      <c r="B56" s="17" t="s">
+      <c r="C56" s="23" t="s">
         <v>351</v>
       </c>
-      <c r="C56" s="23" t="s">
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="23" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="23" t="s">
+      <c r="B57" s="17" t="s">
         <v>353</v>
       </c>
-      <c r="B57" s="17" t="s">
+      <c r="C57" s="23" t="s">
         <v>354</v>
       </c>
-      <c r="C57" s="23" t="s">
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="23" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="23" t="s">
+      <c r="B58" s="17" t="s">
         <v>356</v>
       </c>
-      <c r="B58" s="17" t="s">
+      <c r="C58" s="23" t="s">
         <v>357</v>
       </c>
-      <c r="C58" s="23" t="s">
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="23" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="23" t="s">
+      <c r="B59" s="17" t="s">
         <v>359</v>
       </c>
-      <c r="B59" s="17" t="s">
+      <c r="C59" s="23" t="s">
         <v>360</v>
       </c>
-      <c r="C59" s="23" t="s">
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="23" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="23" t="s">
+      <c r="B60" s="17" t="s">
         <v>362</v>
       </c>
-      <c r="B60" s="17" t="s">
+      <c r="C60" s="23" t="s">
         <v>363</v>
       </c>
-      <c r="C60" s="23" t="s">
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="23" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="23" t="s">
+      <c r="B61" s="17" t="s">
         <v>365</v>
       </c>
-      <c r="B61" s="17" t="s">
+      <c r="C61" s="23" t="s">
         <v>366</v>
       </c>
-      <c r="C61" s="23" t="s">
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="23" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="23" t="s">
+      <c r="B62" s="17" t="s">
         <v>368</v>
       </c>
-      <c r="B62" s="17" t="s">
+      <c r="C62" s="23" t="s">
         <v>369</v>
       </c>
-      <c r="C62" s="23" t="s">
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="23" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="23" t="s">
+      <c r="B63" s="17" t="s">
         <v>371</v>
       </c>
-      <c r="B63" s="17" t="s">
+      <c r="C63" s="23" t="s">
         <v>372</v>
       </c>
-      <c r="C63" s="23" t="s">
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="23" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="23" t="s">
+      <c r="B64" s="17" t="s">
         <v>374</v>
       </c>
-      <c r="B64" s="17" t="s">
+      <c r="C64" s="23" t="s">
         <v>375</v>
       </c>
-      <c r="C64" s="23" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="23"/>
       <c r="B65" s="23"/>
       <c r="C65" s="23" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="23" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="23" t="s">
+      <c r="B66" s="17" t="s">
         <v>378</v>
       </c>
-      <c r="B66" s="17" t="s">
+      <c r="C66" s="23" t="s">
         <v>379</v>
       </c>
-      <c r="C66" s="23" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="23"/>
       <c r="B67" s="23"/>
       <c r="C67" s="23" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="23" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="23" t="s">
+      <c r="B68" s="17" t="s">
         <v>382</v>
       </c>
-      <c r="B68" s="17" t="s">
+      <c r="C68" s="23" t="s">
         <v>383</v>
       </c>
-      <c r="C68" s="23" t="s">
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="23" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="23" t="s">
+      <c r="B69" s="17" t="s">
         <v>385</v>
       </c>
-      <c r="B69" s="17" t="s">
+      <c r="C69" s="23" t="s">
         <v>386</v>
       </c>
-      <c r="C69" s="23" t="s">
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="23" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="23" t="s">
+      <c r="B70" s="17" t="s">
         <v>388</v>
       </c>
-      <c r="B70" s="17" t="s">
+      <c r="C70" s="23" t="s">
         <v>389</v>
       </c>
-      <c r="C70" s="23" t="s">
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="23" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="23" t="s">
+      <c r="B71" s="17" t="s">
         <v>391</v>
       </c>
-      <c r="B71" s="17" t="s">
+      <c r="C71" s="23" t="s">
         <v>392</v>
       </c>
-      <c r="C71" s="23" t="s">
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="23" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="23" t="s">
+      <c r="B72" s="17" t="s">
         <v>394</v>
       </c>
-      <c r="B72" s="17" t="s">
+      <c r="C72" s="23" t="s">
         <v>395</v>
       </c>
-      <c r="C72" s="23" t="s">
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="23" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="23" t="s">
+      <c r="B73" s="17" t="s">
         <v>397</v>
       </c>
-      <c r="B73" s="17" t="s">
+      <c r="C73" s="23" t="s">
         <v>398</v>
       </c>
-      <c r="C73" s="23" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="23"/>
       <c r="B74" s="23"/>
       <c r="C74" s="23" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="23" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="23" t="s">
+      <c r="B75" s="17" t="s">
         <v>401</v>
       </c>
-      <c r="B75" s="17" t="s">
+      <c r="C75" s="23" t="s">
         <v>402</v>
       </c>
-      <c r="C75" s="23" t="s">
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="23" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" s="23" t="s">
+      <c r="B76" s="17" t="s">
         <v>404</v>
       </c>
-      <c r="B76" s="17" t="s">
+      <c r="C76" s="23" t="s">
         <v>405</v>
       </c>
-      <c r="C76" s="23" t="s">
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="23" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" s="23" t="s">
+      <c r="B77" s="17" t="s">
         <v>407</v>
       </c>
-      <c r="B77" s="17" t="s">
+      <c r="C77" s="23" t="s">
         <v>408</v>
       </c>
-      <c r="C77" s="23" t="s">
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="23" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" s="23" t="s">
+      <c r="B78" s="17" t="s">
         <v>410</v>
       </c>
-      <c r="B78" s="17" t="s">
+      <c r="C78" s="23" t="s">
         <v>411</v>
       </c>
-      <c r="C78" s="23" t="s">
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="23" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" s="23" t="s">
+      <c r="B79" s="17" t="s">
         <v>413</v>
       </c>
-      <c r="B79" s="17" t="s">
+      <c r="C79" s="23" t="s">
         <v>414</v>
       </c>
-      <c r="C79" s="23" t="s">
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="23" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" s="23" t="s">
+      <c r="B80" s="17" t="s">
         <v>416</v>
       </c>
-      <c r="B80" s="17" t="s">
+      <c r="C80" s="23" t="s">
         <v>417</v>
       </c>
-      <c r="C80" s="23" t="s">
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="B81" s="23" t="s">
+        <v>246</v>
+      </c>
+      <c r="C81" s="23" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
-      <c r="A81" s="23" t="s">
-        <v>245</v>
-      </c>
-      <c r="B81" s="23" t="s">
-        <v>247</v>
-      </c>
-      <c r="C81" s="23" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="23"/>
       <c r="B82" s="23"/>
       <c r="C82" s="23" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="23"/>
       <c r="B83" s="23"/>
       <c r="C83" s="23" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="23" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="A84" s="23" t="s">
+      <c r="B84" s="17" t="s">
         <v>422</v>
       </c>
-      <c r="B84" s="17" t="s">
+      <c r="C84" s="23" t="s">
         <v>423</v>
       </c>
-      <c r="C84" s="23" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="23"/>
       <c r="B85" s="23"/>
       <c r="C85" s="23" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="23" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86" s="23" t="s">
+      <c r="B86" s="17" t="s">
         <v>426</v>
       </c>
-      <c r="B86" s="17" t="s">
+      <c r="C86" s="23" t="s">
         <v>427</v>
       </c>
-      <c r="C86" s="23" t="s">
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="23" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87" s="23" t="s">
+      <c r="B87" s="17" t="s">
         <v>429</v>
       </c>
-      <c r="B87" s="17" t="s">
+      <c r="C87" s="23" t="s">
         <v>430</v>
       </c>
-      <c r="C87" s="23" t="s">
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="23" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88" s="23" t="s">
+      <c r="B88" s="17" t="s">
         <v>432</v>
       </c>
-      <c r="B88" s="17" t="s">
+      <c r="C88" s="23" t="s">
         <v>433</v>
       </c>
-      <c r="C88" s="23" t="s">
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="23" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="A89" s="23" t="s">
+      <c r="B89" s="17" t="s">
         <v>435</v>
       </c>
-      <c r="B89" s="17" t="s">
+      <c r="C89" s="23" t="s">
         <v>436</v>
       </c>
-      <c r="C89" s="23" t="s">
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="23" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90" s="23" t="s">
+      <c r="B90" s="17" t="s">
         <v>438</v>
       </c>
-      <c r="B90" s="17" t="s">
+      <c r="C90" s="23" t="s">
         <v>439</v>
       </c>
-      <c r="C90" s="23" t="s">
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="23" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="A91" s="23" t="s">
+      <c r="B91" s="17" t="s">
         <v>441</v>
       </c>
-      <c r="B91" s="17" t="s">
+      <c r="C91" s="23" t="s">
         <v>442</v>
       </c>
-      <c r="C91" s="23" t="s">
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="23" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="A92" s="23" t="s">
+      <c r="B92" s="17" t="s">
         <v>444</v>
       </c>
-      <c r="B92" s="17" t="s">
+      <c r="C92" s="23" t="s">
         <v>445</v>
       </c>
-      <c r="C92" s="23" t="s">
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="23" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="93" spans="1:3">
-      <c r="A93" s="23" t="s">
+      <c r="B93" s="17" t="s">
         <v>447</v>
       </c>
-      <c r="B93" s="17" t="s">
+      <c r="C93" s="23" t="s">
         <v>448</v>
       </c>
-      <c r="C93" s="23" t="s">
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="23" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="94" spans="1:3">
-      <c r="A94" s="23" t="s">
+      <c r="B94" s="17" t="s">
         <v>450</v>
       </c>
-      <c r="B94" s="17" t="s">
+      <c r="C94" s="23" t="s">
         <v>451</v>
       </c>
-      <c r="C94" s="23" t="s">
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="23" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="95" spans="1:3">
-      <c r="A95" s="23" t="s">
+      <c r="B95" s="17" t="s">
         <v>453</v>
       </c>
-      <c r="B95" s="17" t="s">
+      <c r="C95" s="23" t="s">
         <v>454</v>
-      </c>
-      <c r="C95" s="23" t="s">
-        <v>455</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{E797F548-F139-4268-A9DA-92B2921EB1F0}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{85B72F49-98BF-4501-A4DA-D86F03A48B31}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{19787057-0BC6-4F49-ACD4-BB7A01990081}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{B2958A65-AD01-45D1-AD7E-A723CE39B18F}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{06CC88DE-E24B-445C-B0F4-83E63C456EFF}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{F0DF9CB1-B935-4679-9453-314424C5B575}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{F6D98B92-B6B3-47A1-9748-AA0503383AB2}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{C6E7B81C-68F2-488F-99FD-7FB2AFD8CFD2}"/>
-    <hyperlink ref="B10" r:id="rId9" xr:uid="{A9EF91F5-EAF8-4028-811A-089B8ADE842F}"/>
-    <hyperlink ref="B11" r:id="rId10" xr:uid="{385DD8EB-E31F-4707-9E65-B8B98A3D3A12}"/>
-    <hyperlink ref="B13" r:id="rId11" xr:uid="{BFDCEF4B-56EC-4CA3-9890-8EFFE544EBD5}"/>
-    <hyperlink ref="B16" r:id="rId12" xr:uid="{7D66AA30-8803-4630-835C-21FE449A1DD2}"/>
-    <hyperlink ref="B17" r:id="rId13" xr:uid="{922E7F08-8B5C-4FA1-AB9A-8D76D25AD3AE}"/>
-    <hyperlink ref="B18" r:id="rId14" xr:uid="{D39E78B5-996B-4720-8394-E9B3829B6ED1}"/>
-    <hyperlink ref="B19" r:id="rId15" xr:uid="{87C847CA-A2FF-41C2-B30D-177D1A653FE2}"/>
-    <hyperlink ref="B20" r:id="rId16" xr:uid="{BB958EEB-5A0E-4E1D-96B8-78B2483B483C}"/>
-    <hyperlink ref="B21" r:id="rId17" xr:uid="{748E97EF-285D-44DC-BB8D-358EE7144BD6}"/>
-    <hyperlink ref="B22" r:id="rId18" xr:uid="{FC88B197-3BF5-49AC-88B3-CD97D94BB7CF}"/>
-    <hyperlink ref="B23" r:id="rId19" xr:uid="{291855FB-6D22-4338-933C-D8A49B78E82B}"/>
-    <hyperlink ref="B24" r:id="rId20" xr:uid="{EBAAD8FD-246B-43F8-BCAC-ADB1A89139DC}"/>
-    <hyperlink ref="B26" r:id="rId21" xr:uid="{7516E568-5615-44C9-A4DE-44C22E9E508B}"/>
-    <hyperlink ref="B27" r:id="rId22" xr:uid="{21285C01-CCBA-4185-93E8-302DCD3C65D9}"/>
-    <hyperlink ref="B28" r:id="rId23" xr:uid="{A8489C91-13DE-42D4-AA7C-60B855F5F962}"/>
-    <hyperlink ref="B29" r:id="rId24" xr:uid="{E52238C5-5AF2-41FF-9926-AD82DC25038D}"/>
-    <hyperlink ref="B30" r:id="rId25" xr:uid="{781B22E7-55EE-4927-B3D2-EE2CBD3CEBC9}"/>
-    <hyperlink ref="B32" r:id="rId26" xr:uid="{CB4F36CD-5D8E-4959-86CB-391E9A578CEB}"/>
-    <hyperlink ref="B33" r:id="rId27" xr:uid="{223593EE-9756-48F9-AA3F-E45A2C88F0FC}"/>
-    <hyperlink ref="B34" r:id="rId28" xr:uid="{1F057BBC-C360-4D4B-B2F6-DC03A6C687D9}"/>
-    <hyperlink ref="B35" r:id="rId29" xr:uid="{E1C8A9DF-50B1-48FC-972F-AB9FAFD85AF1}"/>
-    <hyperlink ref="B36" r:id="rId30" xr:uid="{04700A09-10F7-4C74-A733-B92FF9447C1D}"/>
-    <hyperlink ref="B37" r:id="rId31" xr:uid="{1B3CA46F-30C1-43AB-A42E-E4894AAABB2A}"/>
-    <hyperlink ref="B38" r:id="rId32" xr:uid="{C029512F-16AE-4D11-88B0-C7996C1845B4}"/>
-    <hyperlink ref="B39" r:id="rId33" xr:uid="{70370612-D573-4A20-A842-F496D3FAF775}"/>
-    <hyperlink ref="B41" r:id="rId34" xr:uid="{7BECBEDC-12BF-4568-AAD2-2EC190F91C63}"/>
-    <hyperlink ref="B42" r:id="rId35" xr:uid="{44F8CEFE-523C-4A03-B745-209FE50C2EDC}"/>
-    <hyperlink ref="B43" r:id="rId36" xr:uid="{7560523B-DA22-4054-B9FB-7A3FAAF00A8E}"/>
-    <hyperlink ref="B44" r:id="rId37" xr:uid="{0C022D54-2A7F-4D04-B5F7-0F93FDD09B71}"/>
-    <hyperlink ref="B45" r:id="rId38" xr:uid="{E343C621-82F3-4EB3-8BDD-A3D207AA46B2}"/>
-    <hyperlink ref="B46" r:id="rId39" xr:uid="{C86F74EA-52A1-4E56-B02A-47C97C91B286}"/>
-    <hyperlink ref="B47" r:id="rId40" xr:uid="{44030588-1F00-42EF-BE39-D4E8B5D5A0B9}"/>
-    <hyperlink ref="B48" r:id="rId41" xr:uid="{1240C1E1-45BC-49F1-9177-37D2C939054D}"/>
-    <hyperlink ref="B49" r:id="rId42" xr:uid="{3A00DFBF-A015-4FA8-AA2A-20B5B2A9A635}"/>
-    <hyperlink ref="B50" r:id="rId43" xr:uid="{F40F9D8E-63E7-4DDC-99CA-6858C1A67014}"/>
-    <hyperlink ref="B52" r:id="rId44" xr:uid="{B04F8527-98BC-433F-B04A-CE6021E4F7F1}"/>
-    <hyperlink ref="B53" r:id="rId45" xr:uid="{2659113B-2179-458A-98EB-6B0922D6DDF1}"/>
-    <hyperlink ref="B54" r:id="rId46" xr:uid="{F0E5CF3A-ACD6-491B-B663-3141B2B9278A}"/>
-    <hyperlink ref="B55" r:id="rId47" xr:uid="{8F99E121-6B1F-4F2D-A232-32DE2D96080C}"/>
-    <hyperlink ref="B56" r:id="rId48" xr:uid="{A2EE5EDA-C86C-412E-9C74-1473EF221EEE}"/>
-    <hyperlink ref="B57" r:id="rId49" xr:uid="{AEC0BCCE-2C11-4C8C-99F8-D1F40D103410}"/>
-    <hyperlink ref="B58" r:id="rId50" xr:uid="{D45C22E5-D423-4C0C-9B66-5703CA7F3E96}"/>
-    <hyperlink ref="B59" r:id="rId51" xr:uid="{320B255D-F180-45D7-893E-949CCEF68B17}"/>
-    <hyperlink ref="B60" r:id="rId52" xr:uid="{28B30ED0-F7EC-410B-8F41-98E86F3D06DA}"/>
-    <hyperlink ref="B61" r:id="rId53" xr:uid="{46D01945-A61D-4E1F-B1DD-D2E1B6FAE473}"/>
-    <hyperlink ref="B62" r:id="rId54" xr:uid="{34BECBD0-8A64-4979-9AC1-D72C9F43CFC4}"/>
-    <hyperlink ref="B63" r:id="rId55" xr:uid="{35487386-D64E-4DF6-BDE7-9EB5364155E8}"/>
-    <hyperlink ref="B64" r:id="rId56" xr:uid="{939290E3-7713-47B3-9AC7-25CC7A379DC4}"/>
-    <hyperlink ref="B66" r:id="rId57" xr:uid="{8D5B7703-7410-4133-99DD-CABEFE21A0D7}"/>
-    <hyperlink ref="B68" r:id="rId58" xr:uid="{BE9904C6-D072-4651-8724-736023C5FB09}"/>
-    <hyperlink ref="B69" r:id="rId59" xr:uid="{54C50D78-5298-44E4-BF54-2DF0B5F206A9}"/>
-    <hyperlink ref="B70" r:id="rId60" xr:uid="{755FFD1D-5B48-4A7F-A2E9-7705EAEDB056}"/>
-    <hyperlink ref="B71" r:id="rId61" xr:uid="{9B0B220A-8728-4DAC-90CC-B88EEDFD4D31}"/>
-    <hyperlink ref="B72" r:id="rId62" xr:uid="{63FABCDC-5852-40AC-AF12-4841453180C1}"/>
-    <hyperlink ref="B73" r:id="rId63" xr:uid="{1EEE8E1D-4C78-41EA-A07B-77C067E0EDEC}"/>
-    <hyperlink ref="B75" r:id="rId64" xr:uid="{D2BE4685-22DB-4605-A34C-477E6ED265EA}"/>
-    <hyperlink ref="B76" r:id="rId65" xr:uid="{AEDBE957-9B3F-4A1D-AD4D-EEB2AC5DD93A}"/>
-    <hyperlink ref="B77" r:id="rId66" xr:uid="{39EDFEF3-BA63-4690-ACFE-62C9C8856F0A}"/>
-    <hyperlink ref="B78" r:id="rId67" xr:uid="{823CFED0-536A-4658-950C-85D4EE2BB717}"/>
-    <hyperlink ref="B79" r:id="rId68" xr:uid="{C17EC5DD-392F-4932-9390-9707ECCFB2BC}"/>
-    <hyperlink ref="B80" r:id="rId69" xr:uid="{377C46ED-3FE3-4428-84B6-AB6D547C431E}"/>
-    <hyperlink ref="B84" r:id="rId70" xr:uid="{754EADBC-1031-4665-9A57-B874A1961395}"/>
-    <hyperlink ref="B86" r:id="rId71" xr:uid="{B46EBE10-0D88-4A72-AF6B-24AFD15B6EA1}"/>
-    <hyperlink ref="B87" r:id="rId72" xr:uid="{F83F9755-8C89-4748-97F6-1F6A9089A326}"/>
-    <hyperlink ref="B88" r:id="rId73" xr:uid="{09B5520A-F789-4BC5-9AA0-E15225952DF9}"/>
-    <hyperlink ref="B89" r:id="rId74" xr:uid="{5EFDC6B8-764D-4DFE-9FC3-C6343FF9EDCD}"/>
-    <hyperlink ref="B90" r:id="rId75" xr:uid="{B59BC71E-DB4D-48CC-839A-621FBEC9894C}"/>
-    <hyperlink ref="B91" r:id="rId76" xr:uid="{1A03ED59-7A3F-47AE-9D56-C4D072A3F931}"/>
-    <hyperlink ref="B92" r:id="rId77" xr:uid="{1577D10C-2498-4B1F-A378-CC843AC6EEA8}"/>
-    <hyperlink ref="B93" r:id="rId78" xr:uid="{6D60F907-96CD-4435-82A9-3563341C5819}"/>
-    <hyperlink ref="B94" r:id="rId79" xr:uid="{AE93FA12-B457-43C7-BD39-CF2B8539E9E0}"/>
-    <hyperlink ref="B95" r:id="rId80" xr:uid="{B8A4038A-9BDD-4B9B-869A-0966B2B1060B}"/>
+    <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B9" r:id="rId8"/>
+    <hyperlink ref="B10" r:id="rId9"/>
+    <hyperlink ref="B11" r:id="rId10"/>
+    <hyperlink ref="B13" r:id="rId11"/>
+    <hyperlink ref="B16" r:id="rId12"/>
+    <hyperlink ref="B17" r:id="rId13"/>
+    <hyperlink ref="B18" r:id="rId14"/>
+    <hyperlink ref="B19" r:id="rId15"/>
+    <hyperlink ref="B20" r:id="rId16"/>
+    <hyperlink ref="B21" r:id="rId17"/>
+    <hyperlink ref="B22" r:id="rId18"/>
+    <hyperlink ref="B23" r:id="rId19"/>
+    <hyperlink ref="B24" r:id="rId20"/>
+    <hyperlink ref="B26" r:id="rId21"/>
+    <hyperlink ref="B27" r:id="rId22"/>
+    <hyperlink ref="B28" r:id="rId23"/>
+    <hyperlink ref="B29" r:id="rId24"/>
+    <hyperlink ref="B30" r:id="rId25"/>
+    <hyperlink ref="B32" r:id="rId26"/>
+    <hyperlink ref="B33" r:id="rId27"/>
+    <hyperlink ref="B34" r:id="rId28"/>
+    <hyperlink ref="B35" r:id="rId29"/>
+    <hyperlink ref="B36" r:id="rId30"/>
+    <hyperlink ref="B37" r:id="rId31"/>
+    <hyperlink ref="B38" r:id="rId32"/>
+    <hyperlink ref="B39" r:id="rId33"/>
+    <hyperlink ref="B41" r:id="rId34"/>
+    <hyperlink ref="B42" r:id="rId35"/>
+    <hyperlink ref="B43" r:id="rId36"/>
+    <hyperlink ref="B44" r:id="rId37"/>
+    <hyperlink ref="B45" r:id="rId38"/>
+    <hyperlink ref="B46" r:id="rId39"/>
+    <hyperlink ref="B47" r:id="rId40"/>
+    <hyperlink ref="B48" r:id="rId41"/>
+    <hyperlink ref="B49" r:id="rId42"/>
+    <hyperlink ref="B50" r:id="rId43"/>
+    <hyperlink ref="B52" r:id="rId44"/>
+    <hyperlink ref="B53" r:id="rId45"/>
+    <hyperlink ref="B54" r:id="rId46"/>
+    <hyperlink ref="B55" r:id="rId47"/>
+    <hyperlink ref="B56" r:id="rId48"/>
+    <hyperlink ref="B57" r:id="rId49"/>
+    <hyperlink ref="B58" r:id="rId50"/>
+    <hyperlink ref="B59" r:id="rId51"/>
+    <hyperlink ref="B60" r:id="rId52"/>
+    <hyperlink ref="B61" r:id="rId53"/>
+    <hyperlink ref="B62" r:id="rId54"/>
+    <hyperlink ref="B63" r:id="rId55"/>
+    <hyperlink ref="B64" r:id="rId56"/>
+    <hyperlink ref="B66" r:id="rId57"/>
+    <hyperlink ref="B68" r:id="rId58"/>
+    <hyperlink ref="B69" r:id="rId59"/>
+    <hyperlink ref="B70" r:id="rId60"/>
+    <hyperlink ref="B71" r:id="rId61"/>
+    <hyperlink ref="B72" r:id="rId62"/>
+    <hyperlink ref="B73" r:id="rId63"/>
+    <hyperlink ref="B75" r:id="rId64"/>
+    <hyperlink ref="B76" r:id="rId65"/>
+    <hyperlink ref="B77" r:id="rId66"/>
+    <hyperlink ref="B78" r:id="rId67"/>
+    <hyperlink ref="B79" r:id="rId68"/>
+    <hyperlink ref="B80" r:id="rId69"/>
+    <hyperlink ref="B84" r:id="rId70"/>
+    <hyperlink ref="B86" r:id="rId71"/>
+    <hyperlink ref="B87" r:id="rId72"/>
+    <hyperlink ref="B88" r:id="rId73"/>
+    <hyperlink ref="B89" r:id="rId74"/>
+    <hyperlink ref="B90" r:id="rId75"/>
+    <hyperlink ref="B91" r:id="rId76"/>
+    <hyperlink ref="B92" r:id="rId77"/>
+    <hyperlink ref="B93" r:id="rId78"/>
+    <hyperlink ref="B94" r:id="rId79"/>
+    <hyperlink ref="B95" r:id="rId80"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>